<commit_message>
adding new forecasts for NDMA pilot regions last observed date 18-3-25
</commit_message>
<xml_diff>
--- a/passage_clusters/VIIRS/Kenya/VCI3M_Forecast_Overview_Kenya.xlsx
+++ b/passage_clusters/VIIRS/Kenya/VCI3M_Forecast_Overview_Kenya.xlsx
@@ -535,37 +535,37 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="B1" s="1">
-        <v>45727</v>
+        <v>45734</v>
       </c>
       <c r="C1" s="1">
-        <v>45734</v>
+        <v>45741</v>
       </c>
       <c r="D1" s="1">
-        <v>45741</v>
+        <v>45748</v>
       </c>
       <c r="E1" s="1">
-        <v>45748</v>
+        <v>45755</v>
       </c>
       <c r="F1" s="1">
-        <v>45755</v>
+        <v>45762</v>
       </c>
       <c r="G1" s="1">
-        <v>45762</v>
+        <v>45769</v>
       </c>
       <c r="H1" s="1">
-        <v>45769</v>
+        <v>45776</v>
       </c>
       <c r="I1" s="1">
-        <v>45776</v>
+        <v>45783</v>
       </c>
       <c r="J1" s="1">
-        <v>45783</v>
+        <v>45790</v>
       </c>
       <c r="K1" s="1">
-        <v>45790</v>
+        <v>45797</v>
       </c>
       <c r="L1" s="1">
-        <v>45797</v>
+        <v>45804</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -573,37 +573,37 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>47</v>
+        <v>46.5</v>
       </c>
       <c r="C2">
-        <v>46.3</v>
+        <v>46</v>
       </c>
       <c r="D2">
         <v>45.6</v>
       </c>
       <c r="E2">
-        <v>44.9</v>
+        <v>45.5</v>
       </c>
       <c r="F2">
-        <v>44.4</v>
+        <v>45.8</v>
       </c>
       <c r="G2">
-        <v>44.2</v>
+        <v>46.3</v>
       </c>
       <c r="H2">
-        <v>44.2</v>
+        <v>47.1</v>
       </c>
       <c r="I2">
-        <v>44.3</v>
+        <v>48</v>
       </c>
       <c r="J2">
-        <v>44.6</v>
+        <v>48.9</v>
       </c>
       <c r="K2">
-        <v>44.9</v>
+        <v>49.8</v>
       </c>
       <c r="L2">
-        <v>45.2</v>
+        <v>50.6</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -611,37 +611,37 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>59.2</v>
+        <v>58.8</v>
       </c>
       <c r="C3">
-        <v>58.5</v>
+        <v>58.4</v>
       </c>
       <c r="D3">
-        <v>57.8</v>
+        <v>58.2</v>
       </c>
       <c r="E3">
-        <v>57.1</v>
+        <v>58.2</v>
       </c>
       <c r="F3">
-        <v>56.6</v>
+        <v>58.6</v>
       </c>
       <c r="G3">
-        <v>56.1</v>
+        <v>59</v>
       </c>
       <c r="H3">
-        <v>55.7</v>
+        <v>59.5</v>
       </c>
       <c r="I3">
-        <v>55.2</v>
+        <v>59.9</v>
       </c>
       <c r="J3">
-        <v>54.6</v>
+        <v>60.1</v>
       </c>
       <c r="K3">
-        <v>53.8</v>
+        <v>59.9</v>
       </c>
       <c r="L3">
-        <v>52.7</v>
+        <v>59.5</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -649,37 +649,37 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>21.6</v>
+        <v>23</v>
       </c>
       <c r="C4">
-        <v>22.8</v>
+        <v>25</v>
       </c>
       <c r="D4">
-        <v>24.5</v>
+        <v>27.6</v>
       </c>
       <c r="E4">
-        <v>26.8</v>
+        <v>30.9</v>
       </c>
       <c r="F4">
-        <v>29.5</v>
+        <v>34.5</v>
       </c>
       <c r="G4">
-        <v>32.5</v>
+        <v>38.2</v>
       </c>
       <c r="H4">
-        <v>35.6</v>
+        <v>41.9</v>
       </c>
       <c r="I4">
-        <v>38.5</v>
+        <v>45.4</v>
       </c>
       <c r="J4">
-        <v>41.2</v>
+        <v>48.5</v>
       </c>
       <c r="K4">
-        <v>43.5</v>
+        <v>51.2</v>
       </c>
       <c r="L4">
-        <v>45.4</v>
+        <v>53.3</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -687,37 +687,37 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>37.2</v>
+        <v>38.2</v>
       </c>
       <c r="C5">
-        <v>37.8</v>
+        <v>39.6</v>
       </c>
       <c r="D5">
-        <v>38.8</v>
+        <v>41.5</v>
       </c>
       <c r="E5">
-        <v>40.1</v>
+        <v>44</v>
       </c>
       <c r="F5">
-        <v>41.8</v>
+        <v>46.8</v>
       </c>
       <c r="G5">
-        <v>43.7</v>
+        <v>49.9</v>
       </c>
       <c r="H5">
-        <v>45.6</v>
+        <v>53</v>
       </c>
       <c r="I5">
-        <v>47.5</v>
+        <v>56</v>
       </c>
       <c r="J5">
-        <v>49.2</v>
+        <v>58.7</v>
       </c>
       <c r="K5">
-        <v>50.6</v>
+        <v>60.9</v>
       </c>
       <c r="L5">
-        <v>51.6</v>
+        <v>62.5</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -725,37 +725,37 @@
         <v>4</v>
       </c>
       <c r="B6">
+        <v>49.3</v>
+      </c>
+      <c r="C6">
+        <v>49.1</v>
+      </c>
+      <c r="D6">
+        <v>49.1</v>
+      </c>
+      <c r="E6">
+        <v>49.4</v>
+      </c>
+      <c r="F6">
         <v>49.8</v>
       </c>
-      <c r="C6">
-        <v>49.2</v>
-      </c>
-      <c r="D6">
-        <v>48.7</v>
-      </c>
-      <c r="E6">
-        <v>48.5</v>
-      </c>
-      <c r="F6">
-        <v>48.4</v>
-      </c>
       <c r="G6">
-        <v>48.4</v>
+        <v>50.1</v>
       </c>
       <c r="H6">
-        <v>48.1</v>
+        <v>50.1</v>
       </c>
       <c r="I6">
-        <v>47.5</v>
+        <v>49.7</v>
       </c>
       <c r="J6">
-        <v>46.5</v>
+        <v>48.9</v>
       </c>
       <c r="K6">
-        <v>45.1</v>
+        <v>47.7</v>
       </c>
       <c r="L6">
-        <v>43.4</v>
+        <v>46.2</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -763,37 +763,37 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>31.2</v>
+        <v>34</v>
       </c>
       <c r="C7">
-        <v>33.9</v>
+        <v>37.2</v>
       </c>
       <c r="D7">
-        <v>36.8</v>
+        <v>40.6</v>
       </c>
       <c r="E7">
-        <v>40</v>
+        <v>44.2</v>
       </c>
       <c r="F7">
-        <v>43.2</v>
+        <v>47.8</v>
       </c>
       <c r="G7">
-        <v>46.3</v>
+        <v>51.3</v>
       </c>
       <c r="H7">
-        <v>49.2</v>
+        <v>54.4</v>
       </c>
       <c r="I7">
-        <v>51.7</v>
+        <v>57</v>
       </c>
       <c r="J7">
-        <v>53.7</v>
+        <v>59.1</v>
       </c>
       <c r="K7">
-        <v>55.1</v>
+        <v>60.5</v>
       </c>
       <c r="L7">
-        <v>55.9</v>
+        <v>61.1</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -801,37 +801,37 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>38</v>
+        <v>37.1</v>
       </c>
       <c r="C8">
+        <v>36.7</v>
+      </c>
+      <c r="D8">
         <v>36.9</v>
       </c>
-      <c r="D8">
-        <v>36.1</v>
-      </c>
       <c r="E8">
-        <v>35.8</v>
+        <v>37.8</v>
       </c>
       <c r="F8">
-        <v>36.2</v>
+        <v>39.3</v>
       </c>
       <c r="G8">
-        <v>37</v>
+        <v>41.3</v>
       </c>
       <c r="H8">
-        <v>38.1</v>
+        <v>43.6</v>
       </c>
       <c r="I8">
-        <v>39.5</v>
+        <v>45.9</v>
       </c>
       <c r="J8">
-        <v>40.9</v>
+        <v>48.2</v>
       </c>
       <c r="K8">
-        <v>42.2</v>
+        <v>50.3</v>
       </c>
       <c r="L8">
-        <v>43.4</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -839,37 +839,37 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>55.4</v>
+        <v>53.9</v>
       </c>
       <c r="C9">
-        <v>54.3</v>
+        <v>52.1</v>
       </c>
       <c r="D9">
-        <v>53</v>
+        <v>50.1</v>
       </c>
       <c r="E9">
-        <v>51.7</v>
+        <v>48.2</v>
       </c>
       <c r="F9">
-        <v>50.7</v>
+        <v>46.6</v>
       </c>
       <c r="G9">
-        <v>50.3</v>
+        <v>45.6</v>
       </c>
       <c r="H9">
-        <v>50.6</v>
+        <v>45.1</v>
       </c>
       <c r="I9">
-        <v>51.5</v>
+        <v>45.1</v>
       </c>
       <c r="J9">
-        <v>53.1</v>
+        <v>45.5</v>
       </c>
       <c r="K9">
-        <v>55</v>
+        <v>46.2</v>
       </c>
       <c r="L9">
-        <v>57.1</v>
+        <v>47.1</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -877,37 +877,37 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>46.4</v>
+        <v>45.7</v>
       </c>
       <c r="C10">
-        <v>45.8</v>
+        <v>45</v>
       </c>
       <c r="D10">
-        <v>45.1</v>
+        <v>44.3</v>
       </c>
       <c r="E10">
-        <v>44.6</v>
+        <v>43.8</v>
       </c>
       <c r="F10">
-        <v>44.3</v>
+        <v>43.4</v>
       </c>
       <c r="G10">
+        <v>43.3</v>
+      </c>
+      <c r="H10">
+        <v>43.3</v>
+      </c>
+      <c r="I10">
+        <v>43.5</v>
+      </c>
+      <c r="J10">
+        <v>43.8</v>
+      </c>
+      <c r="K10">
         <v>44.2</v>
       </c>
-      <c r="H10">
-        <v>44.3</v>
-      </c>
-      <c r="I10">
+      <c r="L10">
         <v>44.7</v>
-      </c>
-      <c r="J10">
-        <v>45.1</v>
-      </c>
-      <c r="K10">
-        <v>45.8</v>
-      </c>
-      <c r="L10">
-        <v>46.4</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -915,37 +915,37 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>38.9</v>
+        <v>35.3</v>
       </c>
       <c r="C11">
-        <v>34.8</v>
+        <v>32.2</v>
       </c>
       <c r="D11">
-        <v>31.1</v>
+        <v>29.7</v>
       </c>
       <c r="E11">
+        <v>28.3</v>
+      </c>
+      <c r="F11">
         <v>27.8</v>
       </c>
-      <c r="F11">
-        <v>25.3</v>
-      </c>
       <c r="G11">
-        <v>23.3</v>
+        <v>28</v>
       </c>
       <c r="H11">
-        <v>22</v>
+        <v>29.1</v>
       </c>
       <c r="I11">
-        <v>21.3</v>
+        <v>30.8</v>
       </c>
       <c r="J11">
-        <v>21.1</v>
+        <v>33</v>
       </c>
       <c r="K11">
-        <v>21.5</v>
+        <v>35.6</v>
       </c>
       <c r="L11">
-        <v>22.4</v>
+        <v>38.3</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -953,37 +953,37 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>66.59999999999999</v>
+        <v>66.3</v>
       </c>
       <c r="C12">
-        <v>65.8</v>
+        <v>65.40000000000001</v>
       </c>
       <c r="D12">
-        <v>64.09999999999999</v>
+        <v>63.9</v>
       </c>
       <c r="E12">
-        <v>61.6</v>
+        <v>62</v>
       </c>
       <c r="F12">
-        <v>58.3</v>
+        <v>59.7</v>
       </c>
       <c r="G12">
-        <v>54.3</v>
+        <v>57.1</v>
       </c>
       <c r="H12">
-        <v>49.9</v>
+        <v>54.5</v>
       </c>
       <c r="I12">
-        <v>45.2</v>
+        <v>51.9</v>
       </c>
       <c r="J12">
-        <v>40.4</v>
+        <v>49.4</v>
       </c>
       <c r="K12">
-        <v>35.7</v>
+        <v>47.1</v>
       </c>
       <c r="L12">
-        <v>31.3</v>
+        <v>45.1</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -991,37 +991,37 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>57.1</v>
+        <v>55.3</v>
       </c>
       <c r="C13">
-        <v>55.8</v>
+        <v>53</v>
       </c>
       <c r="D13">
-        <v>54</v>
+        <v>50.3</v>
       </c>
       <c r="E13">
-        <v>52.2</v>
+        <v>47.6</v>
       </c>
       <c r="F13">
-        <v>50.6</v>
+        <v>45.3</v>
       </c>
       <c r="G13">
-        <v>49.6</v>
+        <v>43.4</v>
       </c>
       <c r="H13">
-        <v>49.4</v>
+        <v>42.2</v>
       </c>
       <c r="I13">
-        <v>49.9</v>
+        <v>41.6</v>
       </c>
       <c r="J13">
-        <v>51.1</v>
+        <v>41.6</v>
       </c>
       <c r="K13">
-        <v>52.8</v>
+        <v>42</v>
       </c>
       <c r="L13">
-        <v>54.9</v>
+        <v>42.7</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1029,37 +1029,37 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>40.5</v>
+        <v>37.5</v>
       </c>
       <c r="C14">
-        <v>36.9</v>
+        <v>34.9</v>
       </c>
       <c r="D14">
-        <v>33.3</v>
+        <v>32.8</v>
       </c>
       <c r="E14">
-        <v>30.1</v>
+        <v>31.8</v>
       </c>
       <c r="F14">
-        <v>27.5</v>
+        <v>31.6</v>
       </c>
       <c r="G14">
-        <v>25.4</v>
+        <v>32.5</v>
       </c>
       <c r="H14">
-        <v>24</v>
+        <v>34.2</v>
       </c>
       <c r="I14">
-        <v>23.2</v>
+        <v>36.7</v>
       </c>
       <c r="J14">
-        <v>23.1</v>
+        <v>39.9</v>
       </c>
       <c r="K14">
-        <v>23.7</v>
+        <v>43.4</v>
       </c>
       <c r="L14">
-        <v>24.8</v>
+        <v>47.1</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1067,37 +1067,37 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>56.8</v>
+        <v>54.7</v>
       </c>
       <c r="C15">
-        <v>54.5</v>
+        <v>51.9</v>
       </c>
       <c r="D15">
-        <v>51.7</v>
+        <v>48.8</v>
       </c>
       <c r="E15">
-        <v>48.4</v>
+        <v>45.6</v>
       </c>
       <c r="F15">
-        <v>44.9</v>
+        <v>42.5</v>
       </c>
       <c r="G15">
-        <v>41.5</v>
+        <v>39.7</v>
       </c>
       <c r="H15">
-        <v>38.3</v>
+        <v>37.2</v>
       </c>
       <c r="I15">
-        <v>35.3</v>
+        <v>35.1</v>
       </c>
       <c r="J15">
-        <v>32.8</v>
+        <v>33.4</v>
       </c>
       <c r="K15">
-        <v>30.8</v>
+        <v>32.3</v>
       </c>
       <c r="L15">
-        <v>29.2</v>
+        <v>31.6</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1105,37 +1105,37 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>45.5</v>
+        <v>43.2</v>
       </c>
       <c r="C16">
-        <v>43</v>
+        <v>40.5</v>
       </c>
       <c r="D16">
-        <v>40.1</v>
+        <v>37.6</v>
       </c>
       <c r="E16">
-        <v>37</v>
+        <v>34.6</v>
       </c>
       <c r="F16">
-        <v>33.7</v>
+        <v>31.5</v>
       </c>
       <c r="G16">
-        <v>30.2</v>
+        <v>28.4</v>
       </c>
       <c r="H16">
-        <v>26.5</v>
+        <v>25.1</v>
       </c>
       <c r="I16">
-        <v>22.8</v>
+        <v>22</v>
       </c>
       <c r="J16">
-        <v>19.1</v>
+        <v>18.9</v>
       </c>
       <c r="K16">
-        <v>15.5</v>
+        <v>16.2</v>
       </c>
       <c r="L16">
-        <v>12.2</v>
+        <v>13.9</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1143,37 +1143,37 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>55.6</v>
+        <v>54.2</v>
       </c>
       <c r="C17">
-        <v>54.5</v>
+        <v>52.5</v>
       </c>
       <c r="D17">
-        <v>53.3</v>
+        <v>50.7</v>
       </c>
       <c r="E17">
-        <v>52.1</v>
+        <v>48.9</v>
       </c>
       <c r="F17">
-        <v>51.2</v>
+        <v>47.3</v>
       </c>
       <c r="G17">
-        <v>50.6</v>
+        <v>46</v>
       </c>
       <c r="H17">
-        <v>50.5</v>
+        <v>45</v>
       </c>
       <c r="I17">
-        <v>50.8</v>
+        <v>44.5</v>
       </c>
       <c r="J17">
-        <v>51.7</v>
+        <v>44.3</v>
       </c>
       <c r="K17">
-        <v>52.8</v>
+        <v>44.4</v>
       </c>
       <c r="L17">
-        <v>54.2</v>
+        <v>44.8</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1181,37 +1181,37 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>57.3</v>
+        <v>55.4</v>
       </c>
       <c r="C18">
-        <v>55.7</v>
+        <v>53.2</v>
       </c>
       <c r="D18">
-        <v>53.9</v>
+        <v>50.7</v>
       </c>
       <c r="E18">
-        <v>52.1</v>
+        <v>48.5</v>
       </c>
       <c r="F18">
-        <v>50.6</v>
+        <v>46.6</v>
       </c>
       <c r="G18">
-        <v>49.7</v>
+        <v>45.4</v>
       </c>
       <c r="H18">
-        <v>49.6</v>
+        <v>45</v>
       </c>
       <c r="I18">
-        <v>50.3</v>
+        <v>45.2</v>
       </c>
       <c r="J18">
-        <v>51.9</v>
+        <v>46.1</v>
       </c>
       <c r="K18">
-        <v>54</v>
+        <v>47.5</v>
       </c>
       <c r="L18">
-        <v>56.5</v>
+        <v>49.1</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1219,37 +1219,37 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>47.3</v>
+        <v>45.7</v>
       </c>
       <c r="C19">
-        <v>45.2</v>
+        <v>44</v>
       </c>
       <c r="D19">
-        <v>42.9</v>
+        <v>42.5</v>
       </c>
       <c r="E19">
-        <v>40.4</v>
+        <v>41.2</v>
       </c>
       <c r="F19">
-        <v>38</v>
+        <v>40.3</v>
       </c>
       <c r="G19">
-        <v>35.7</v>
+        <v>39.7</v>
       </c>
       <c r="H19">
-        <v>33.4</v>
+        <v>39.5</v>
       </c>
       <c r="I19">
-        <v>31.4</v>
+        <v>39.5</v>
       </c>
       <c r="J19">
-        <v>29.5</v>
+        <v>39.8</v>
       </c>
       <c r="K19">
-        <v>27.9</v>
+        <v>40.2</v>
       </c>
       <c r="L19">
-        <v>26.6</v>
+        <v>40.8</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1257,37 +1257,37 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>39.9</v>
+        <v>40.9</v>
       </c>
       <c r="C20">
-        <v>41</v>
+        <v>42.4</v>
       </c>
       <c r="D20">
-        <v>42.5</v>
+        <v>44.3</v>
       </c>
       <c r="E20">
-        <v>44.4</v>
+        <v>46.4</v>
       </c>
       <c r="F20">
-        <v>46.6</v>
+        <v>48.7</v>
       </c>
       <c r="G20">
-        <v>48.9</v>
+        <v>50.8</v>
       </c>
       <c r="H20">
-        <v>51.2</v>
+        <v>52.7</v>
       </c>
       <c r="I20">
-        <v>53.2</v>
+        <v>54.1</v>
       </c>
       <c r="J20">
-        <v>54.7</v>
+        <v>55.1</v>
       </c>
       <c r="K20">
-        <v>55.8</v>
+        <v>55.5</v>
       </c>
       <c r="L20">
-        <v>56.3</v>
+        <v>55.4</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1295,37 +1295,37 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>52.3</v>
+        <v>52.9</v>
       </c>
       <c r="C21">
-        <v>52.7</v>
+        <v>53.4</v>
       </c>
       <c r="D21">
-        <v>53.1</v>
+        <v>54</v>
       </c>
       <c r="E21">
-        <v>53.5</v>
+        <v>54.7</v>
       </c>
       <c r="F21">
-        <v>53.8</v>
+        <v>55.3</v>
       </c>
       <c r="G21">
-        <v>54.1</v>
+        <v>55.9</v>
       </c>
       <c r="H21">
-        <v>54.3</v>
+        <v>56.5</v>
       </c>
       <c r="I21">
-        <v>54.4</v>
+        <v>56.8</v>
       </c>
       <c r="J21">
-        <v>54.2</v>
+        <v>56.9</v>
       </c>
       <c r="K21">
-        <v>53.8</v>
+        <v>56.7</v>
       </c>
       <c r="L21">
-        <v>53.1</v>
+        <v>56.2</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1333,37 +1333,37 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>39.5</v>
+        <v>40</v>
       </c>
       <c r="C22">
-        <v>39.6</v>
+        <v>40.8</v>
       </c>
       <c r="D22">
-        <v>39.9</v>
+        <v>42</v>
       </c>
       <c r="E22">
-        <v>40.5</v>
+        <v>43.9</v>
       </c>
       <c r="F22">
-        <v>41.4</v>
+        <v>46.2</v>
       </c>
       <c r="G22">
-        <v>42.6</v>
+        <v>49.1</v>
       </c>
       <c r="H22">
-        <v>44.1</v>
+        <v>52.2</v>
       </c>
       <c r="I22">
-        <v>45.8</v>
+        <v>55.4</v>
       </c>
       <c r="J22">
-        <v>47.5</v>
+        <v>58.4</v>
       </c>
       <c r="K22">
-        <v>49.1</v>
+        <v>61.1</v>
       </c>
       <c r="L22">
-        <v>50.4</v>
+        <v>63.3</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1371,37 +1371,37 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>43.9</v>
+        <v>41.7</v>
       </c>
       <c r="C23">
-        <v>41.2</v>
+        <v>39.8</v>
       </c>
       <c r="D23">
-        <v>38.6</v>
+        <v>38.4</v>
       </c>
       <c r="E23">
-        <v>36.3</v>
+        <v>37.8</v>
       </c>
       <c r="F23">
-        <v>34.6</v>
+        <v>38</v>
       </c>
       <c r="G23">
-        <v>33.3</v>
+        <v>38.9</v>
       </c>
       <c r="H23">
-        <v>32.5</v>
+        <v>40.5</v>
       </c>
       <c r="I23">
-        <v>32.2</v>
+        <v>42.6</v>
       </c>
       <c r="J23">
-        <v>32.3</v>
+        <v>45.1</v>
       </c>
       <c r="K23">
-        <v>32.9</v>
+        <v>47.7</v>
       </c>
       <c r="L23">
-        <v>33.7</v>
+        <v>50.3</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1409,37 +1409,37 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>50.3</v>
+        <v>49.3</v>
       </c>
       <c r="C24">
-        <v>49.8</v>
+        <v>48.1</v>
       </c>
       <c r="D24">
-        <v>49.2</v>
+        <v>46.9</v>
       </c>
       <c r="E24">
-        <v>48.8</v>
+        <v>45.7</v>
       </c>
       <c r="F24">
-        <v>48.7</v>
+        <v>44.6</v>
       </c>
       <c r="G24">
-        <v>49</v>
+        <v>43.8</v>
       </c>
       <c r="H24">
-        <v>49.8</v>
+        <v>43.2</v>
       </c>
       <c r="I24">
-        <v>51</v>
+        <v>42.9</v>
       </c>
       <c r="J24">
-        <v>52.4</v>
+        <v>42.6</v>
       </c>
       <c r="K24">
-        <v>54</v>
+        <v>42.5</v>
       </c>
       <c r="L24">
-        <v>55.6</v>
+        <v>42.5</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -1447,37 +1447,37 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>51.4</v>
+        <v>48.3</v>
       </c>
       <c r="C25">
-        <v>48.2</v>
+        <v>44.8</v>
       </c>
       <c r="D25">
-        <v>44.6</v>
+        <v>41.3</v>
       </c>
       <c r="E25">
-        <v>40.8</v>
+        <v>37.9</v>
       </c>
       <c r="F25">
-        <v>37.1</v>
+        <v>34.7</v>
       </c>
       <c r="G25">
-        <v>33.6</v>
+        <v>31.9</v>
       </c>
       <c r="H25">
-        <v>30.3</v>
+        <v>29.5</v>
       </c>
       <c r="I25">
-        <v>27.5</v>
+        <v>27.6</v>
       </c>
       <c r="J25">
-        <v>25.1</v>
+        <v>26.1</v>
       </c>
       <c r="K25">
-        <v>23.1</v>
+        <v>25</v>
       </c>
       <c r="L25">
-        <v>21.5</v>
+        <v>24.3</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1485,37 +1485,37 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>52.2</v>
+        <v>50.6</v>
       </c>
       <c r="C26">
-        <v>50.7</v>
+        <v>48.8</v>
       </c>
       <c r="D26">
-        <v>49.1</v>
+        <v>47</v>
       </c>
       <c r="E26">
-        <v>47.6</v>
+        <v>45.4</v>
       </c>
       <c r="F26">
-        <v>46.4</v>
+        <v>44.1</v>
       </c>
       <c r="G26">
-        <v>45.5</v>
+        <v>43.2</v>
       </c>
       <c r="H26">
-        <v>45.1</v>
+        <v>42.6</v>
       </c>
       <c r="I26">
-        <v>45.2</v>
+        <v>42.5</v>
       </c>
       <c r="J26">
-        <v>45.7</v>
+        <v>42.8</v>
       </c>
       <c r="K26">
-        <v>46.5</v>
+        <v>43.3</v>
       </c>
       <c r="L26">
-        <v>47.6</v>
+        <v>44.1</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1523,37 +1523,37 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>32.8</v>
+        <v>35.1</v>
       </c>
       <c r="C27">
-        <v>34.7</v>
+        <v>38</v>
       </c>
       <c r="D27">
-        <v>37.1</v>
+        <v>41.5</v>
       </c>
       <c r="E27">
-        <v>39.8</v>
+        <v>45.4</v>
       </c>
       <c r="F27">
-        <v>42.7</v>
+        <v>49.5</v>
       </c>
       <c r="G27">
-        <v>45.7</v>
+        <v>53.7</v>
       </c>
       <c r="H27">
-        <v>48.5</v>
+        <v>57.7</v>
       </c>
       <c r="I27">
-        <v>50.9</v>
+        <v>61.4</v>
       </c>
       <c r="J27">
-        <v>53</v>
+        <v>64.5</v>
       </c>
       <c r="K27">
-        <v>54.5</v>
+        <v>66.90000000000001</v>
       </c>
       <c r="L27">
-        <v>55.4</v>
+        <v>68.59999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -1561,37 +1561,37 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>30.6</v>
+        <v>31.9</v>
       </c>
       <c r="C28">
-        <v>31.9</v>
+        <v>33.8</v>
       </c>
       <c r="D28">
-        <v>33.7</v>
+        <v>36.2</v>
       </c>
       <c r="E28">
-        <v>36.1</v>
+        <v>39.2</v>
       </c>
       <c r="F28">
-        <v>39</v>
+        <v>42.4</v>
       </c>
       <c r="G28">
-        <v>42.1</v>
+        <v>45.7</v>
       </c>
       <c r="H28">
-        <v>45.3</v>
+        <v>48.9</v>
       </c>
       <c r="I28">
-        <v>48.3</v>
+        <v>51.8</v>
       </c>
       <c r="J28">
-        <v>51.1</v>
+        <v>54.2</v>
       </c>
       <c r="K28">
-        <v>53.3</v>
+        <v>56.1</v>
       </c>
       <c r="L28">
-        <v>55</v>
+        <v>57.3</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1599,37 +1599,37 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>35.4</v>
+        <v>36.6</v>
       </c>
       <c r="C29">
-        <v>36.7</v>
+        <v>38.1</v>
       </c>
       <c r="D29">
-        <v>38.4</v>
+        <v>40</v>
       </c>
       <c r="E29">
-        <v>40.6</v>
+        <v>42.3</v>
       </c>
       <c r="F29">
-        <v>43.2</v>
+        <v>44.7</v>
       </c>
       <c r="G29">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H29">
-        <v>48.8</v>
+        <v>49</v>
       </c>
       <c r="I29">
-        <v>51.3</v>
+        <v>50.5</v>
       </c>
       <c r="J29">
-        <v>53.4</v>
+        <v>51.4</v>
       </c>
       <c r="K29">
-        <v>54.9</v>
+        <v>51.8</v>
       </c>
       <c r="L29">
-        <v>55.7</v>
+        <v>51.5</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -1637,37 +1637,37 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>32.1</v>
+        <v>33.2</v>
       </c>
       <c r="C30">
-        <v>33.6</v>
+        <v>34.5</v>
       </c>
       <c r="D30">
-        <v>35.5</v>
+        <v>36</v>
       </c>
       <c r="E30">
-        <v>37.8</v>
+        <v>37.5</v>
       </c>
       <c r="F30">
-        <v>40.3</v>
+        <v>38.9</v>
       </c>
       <c r="G30">
-        <v>43</v>
+        <v>40.2</v>
       </c>
       <c r="H30">
-        <v>45.7</v>
+        <v>41.1</v>
       </c>
       <c r="I30">
-        <v>48.2</v>
+        <v>41.5</v>
       </c>
       <c r="J30">
-        <v>50.4</v>
+        <v>41.6</v>
       </c>
       <c r="K30">
-        <v>52.1</v>
+        <v>41.2</v>
       </c>
       <c r="L30">
-        <v>53.2</v>
+        <v>40.4</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -1675,37 +1675,37 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>60.8</v>
+        <v>59.8</v>
       </c>
       <c r="C31">
-        <v>59.5</v>
+        <v>58.2</v>
       </c>
       <c r="D31">
-        <v>57.6</v>
+        <v>56.2</v>
       </c>
       <c r="E31">
-        <v>55</v>
+        <v>53.7</v>
       </c>
       <c r="F31">
-        <v>51.8</v>
+        <v>50.9</v>
       </c>
       <c r="G31">
-        <v>48.1</v>
+        <v>47.9</v>
       </c>
       <c r="H31">
-        <v>44</v>
+        <v>44.6</v>
       </c>
       <c r="I31">
-        <v>39.7</v>
+        <v>41.2</v>
       </c>
       <c r="J31">
-        <v>35.1</v>
+        <v>37.9</v>
       </c>
       <c r="K31">
-        <v>30.6</v>
+        <v>34.8</v>
       </c>
       <c r="L31">
-        <v>26.4</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -1713,37 +1713,37 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>33.5</v>
+        <v>34.2</v>
       </c>
       <c r="C32">
-        <v>34</v>
+        <v>35.3</v>
       </c>
       <c r="D32">
-        <v>34.7</v>
+        <v>36.8</v>
       </c>
       <c r="E32">
-        <v>35.8</v>
+        <v>38.6</v>
       </c>
       <c r="F32">
-        <v>37.1</v>
+        <v>40.7</v>
       </c>
       <c r="G32">
-        <v>38.5</v>
+        <v>42.8</v>
       </c>
       <c r="H32">
-        <v>39.7</v>
+        <v>44.7</v>
       </c>
       <c r="I32">
-        <v>40.7</v>
+        <v>46.3</v>
       </c>
       <c r="J32">
-        <v>41.4</v>
+        <v>47.5</v>
       </c>
       <c r="K32">
-        <v>41.6</v>
+        <v>48.2</v>
       </c>
       <c r="L32">
-        <v>41.4</v>
+        <v>48.4</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -1751,37 +1751,37 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>65</v>
+        <v>63.8</v>
       </c>
       <c r="C33">
-        <v>63.6</v>
+        <v>61.7</v>
       </c>
       <c r="D33">
-        <v>61.3</v>
+        <v>58.9</v>
       </c>
       <c r="E33">
-        <v>58.4</v>
+        <v>55.8</v>
       </c>
       <c r="F33">
-        <v>54.9</v>
+        <v>52.6</v>
       </c>
       <c r="G33">
-        <v>51.4</v>
+        <v>49.7</v>
       </c>
       <c r="H33">
-        <v>48.1</v>
+        <v>47.3</v>
       </c>
       <c r="I33">
-        <v>45.1</v>
+        <v>45.3</v>
       </c>
       <c r="J33">
+        <v>43.9</v>
+      </c>
+      <c r="K33">
+        <v>43.1</v>
+      </c>
+      <c r="L33">
         <v>42.6</v>
-      </c>
-      <c r="K33">
-        <v>40.7</v>
-      </c>
-      <c r="L33">
-        <v>39.4</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -1789,37 +1789,37 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>47</v>
+        <v>47.8</v>
       </c>
       <c r="C34">
-        <v>46.8</v>
+        <v>49</v>
       </c>
       <c r="D34">
-        <v>46.9</v>
+        <v>51</v>
       </c>
       <c r="E34">
-        <v>47.3</v>
+        <v>54</v>
       </c>
       <c r="F34">
-        <v>48.1</v>
+        <v>57.9</v>
       </c>
       <c r="G34">
-        <v>49.3</v>
+        <v>62.7</v>
       </c>
       <c r="H34">
-        <v>51</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="I34">
-        <v>52.8</v>
+        <v>73.5</v>
       </c>
       <c r="J34">
-        <v>54.8</v>
+        <v>78.8</v>
       </c>
       <c r="K34">
-        <v>56.6</v>
+        <v>83.7</v>
       </c>
       <c r="L34">
-        <v>58.2</v>
+        <v>87.59999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -1827,37 +1827,37 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>46.9</v>
+        <v>43.8</v>
       </c>
       <c r="C35">
-        <v>43.3</v>
+        <v>41</v>
       </c>
       <c r="D35">
-        <v>39.7</v>
+        <v>38.6</v>
       </c>
       <c r="E35">
-        <v>36.4</v>
+        <v>36.9</v>
       </c>
       <c r="F35">
-        <v>33.4</v>
+        <v>36</v>
       </c>
       <c r="G35">
-        <v>30.9</v>
+        <v>35.9</v>
       </c>
       <c r="H35">
-        <v>29</v>
+        <v>36.5</v>
       </c>
       <c r="I35">
-        <v>27.6</v>
+        <v>38</v>
       </c>
       <c r="J35">
-        <v>26.9</v>
+        <v>40</v>
       </c>
       <c r="K35">
-        <v>26.9</v>
+        <v>42.5</v>
       </c>
       <c r="L35">
-        <v>27.4</v>
+        <v>45.2</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -1865,37 +1865,37 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>49.8</v>
+        <v>49.6</v>
       </c>
       <c r="C36">
-        <v>49.8</v>
+        <v>48.8</v>
       </c>
       <c r="D36">
-        <v>49.2</v>
+        <v>47.6</v>
       </c>
       <c r="E36">
-        <v>48.3</v>
+        <v>46</v>
       </c>
       <c r="F36">
-        <v>47.1</v>
+        <v>44.4</v>
       </c>
       <c r="G36">
-        <v>46</v>
+        <v>43.1</v>
       </c>
       <c r="H36">
-        <v>45.2</v>
+        <v>42.2</v>
       </c>
       <c r="I36">
-        <v>44.9</v>
+        <v>41.7</v>
       </c>
       <c r="J36">
-        <v>45.2</v>
+        <v>41.9</v>
       </c>
       <c r="K36">
-        <v>45.9</v>
+        <v>42.5</v>
       </c>
       <c r="L36">
-        <v>47.2</v>
+        <v>43.6</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -1903,37 +1903,37 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>44.6</v>
+        <v>44.5</v>
       </c>
       <c r="C37">
+        <v>44.4</v>
+      </c>
+      <c r="D37">
         <v>44.5</v>
       </c>
-      <c r="D37">
-        <v>44.3</v>
-      </c>
       <c r="E37">
-        <v>44.3</v>
+        <v>44.9</v>
       </c>
       <c r="F37">
-        <v>44.6</v>
+        <v>45.7</v>
       </c>
       <c r="G37">
-        <v>45.3</v>
+        <v>46.8</v>
       </c>
       <c r="H37">
-        <v>46.4</v>
+        <v>48.2</v>
       </c>
       <c r="I37">
-        <v>47.6</v>
+        <v>49.7</v>
       </c>
       <c r="J37">
-        <v>49</v>
+        <v>51.1</v>
       </c>
       <c r="K37">
-        <v>50.2</v>
+        <v>52.2</v>
       </c>
       <c r="L37">
-        <v>51.2</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -1941,37 +1941,37 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>46.7</v>
+        <v>43.8</v>
       </c>
       <c r="C38">
-        <v>43.3</v>
+        <v>41.2</v>
       </c>
       <c r="D38">
-        <v>40.1</v>
+        <v>39.1</v>
       </c>
       <c r="E38">
-        <v>37.2</v>
+        <v>38</v>
       </c>
       <c r="F38">
-        <v>34.9</v>
+        <v>37.7</v>
       </c>
       <c r="G38">
-        <v>33.3</v>
+        <v>38.4</v>
       </c>
       <c r="H38">
-        <v>32.4</v>
+        <v>40</v>
       </c>
       <c r="I38">
-        <v>32.3</v>
+        <v>42.4</v>
       </c>
       <c r="J38">
-        <v>32.8</v>
+        <v>45.2</v>
       </c>
       <c r="K38">
-        <v>33.8</v>
+        <v>48.4</v>
       </c>
       <c r="L38">
-        <v>35.3</v>
+        <v>51.6</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -1979,37 +1979,37 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>30.3</v>
+        <v>31.9</v>
       </c>
       <c r="C39">
-        <v>32.1</v>
+        <v>33.8</v>
       </c>
       <c r="D39">
-        <v>34.4</v>
+        <v>36</v>
       </c>
       <c r="E39">
-        <v>37</v>
+        <v>38.5</v>
       </c>
       <c r="F39">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G39">
-        <v>43.2</v>
+        <v>43.3</v>
       </c>
       <c r="H39">
-        <v>46.3</v>
+        <v>45.3</v>
       </c>
       <c r="I39">
-        <v>49.1</v>
+        <v>46.7</v>
       </c>
       <c r="J39">
-        <v>51.4</v>
+        <v>47.5</v>
       </c>
       <c r="K39">
-        <v>53.1</v>
+        <v>47.7</v>
       </c>
       <c r="L39">
-        <v>54.1</v>
+        <v>47.3</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -2017,37 +2017,37 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C40">
-        <v>75.90000000000001</v>
+        <v>74</v>
       </c>
       <c r="D40">
-        <v>73.8</v>
+        <v>71.2</v>
       </c>
       <c r="E40">
-        <v>70.8</v>
+        <v>68</v>
       </c>
       <c r="F40">
-        <v>67.2</v>
+        <v>64.59999999999999</v>
       </c>
       <c r="G40">
-        <v>63.6</v>
+        <v>61.5</v>
       </c>
       <c r="H40">
-        <v>60.1</v>
+        <v>58.8</v>
       </c>
       <c r="I40">
-        <v>56.9</v>
+        <v>56.5</v>
       </c>
       <c r="J40">
-        <v>54.3</v>
+        <v>54.8</v>
       </c>
       <c r="K40">
-        <v>52.1</v>
+        <v>53.5</v>
       </c>
       <c r="L40">
-        <v>50.4</v>
+        <v>52.5</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -2055,37 +2055,37 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>59.1</v>
+        <v>58.4</v>
       </c>
       <c r="C41">
-        <v>57.9</v>
+        <v>57.8</v>
       </c>
       <c r="D41">
-        <v>56.5</v>
+        <v>57.5</v>
       </c>
       <c r="E41">
-        <v>55.2</v>
+        <v>57.7</v>
       </c>
       <c r="F41">
-        <v>54</v>
+        <v>58.3</v>
       </c>
       <c r="G41">
-        <v>53.1</v>
+        <v>59.6</v>
       </c>
       <c r="H41">
-        <v>52.5</v>
+        <v>61.3</v>
       </c>
       <c r="I41">
-        <v>52.1</v>
+        <v>63.4</v>
       </c>
       <c r="J41">
-        <v>52.1</v>
+        <v>65.8</v>
       </c>
       <c r="K41">
-        <v>52.2</v>
+        <v>68.09999999999999</v>
       </c>
       <c r="L41">
-        <v>52.5</v>
+        <v>70.09999999999999</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -2093,37 +2093,37 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>55</v>
+        <v>53.6</v>
       </c>
       <c r="C42">
-        <v>53.1</v>
+        <v>52.2</v>
       </c>
       <c r="D42">
-        <v>50.9</v>
+        <v>51</v>
       </c>
       <c r="E42">
-        <v>48.9</v>
+        <v>50.5</v>
       </c>
       <c r="F42">
-        <v>47.1</v>
+        <v>50.7</v>
       </c>
       <c r="G42">
-        <v>45.8</v>
+        <v>51.6</v>
       </c>
       <c r="H42">
-        <v>44.9</v>
+        <v>53.3</v>
       </c>
       <c r="I42">
-        <v>44.6</v>
+        <v>55.4</v>
       </c>
       <c r="J42">
-        <v>44.7</v>
+        <v>57.9</v>
       </c>
       <c r="K42">
-        <v>45.1</v>
+        <v>60.4</v>
       </c>
       <c r="L42">
-        <v>45.8</v>
+        <v>62.9</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -2131,37 +2131,37 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>52</v>
+        <v>49.5</v>
       </c>
       <c r="C43">
-        <v>48.6</v>
+        <v>47.4</v>
       </c>
       <c r="D43">
-        <v>45.3</v>
+        <v>46.3</v>
       </c>
       <c r="E43">
-        <v>42.6</v>
+        <v>46.5</v>
       </c>
       <c r="F43">
-        <v>40.7</v>
+        <v>48.1</v>
       </c>
       <c r="G43">
-        <v>39.6</v>
+        <v>51</v>
       </c>
       <c r="H43">
-        <v>39.5</v>
+        <v>55.1</v>
       </c>
       <c r="I43">
-        <v>40.3</v>
+        <v>60.1</v>
       </c>
       <c r="J43">
-        <v>41.8</v>
+        <v>65.5</v>
       </c>
       <c r="K43">
-        <v>43.7</v>
+        <v>71</v>
       </c>
       <c r="L43">
-        <v>46</v>
+        <v>76.09999999999999</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -2169,37 +2169,37 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>53.3</v>
+        <v>51.3</v>
       </c>
       <c r="C44">
-        <v>50.8</v>
+        <v>49.2</v>
       </c>
       <c r="D44">
-        <v>48.1</v>
+        <v>47.4</v>
       </c>
       <c r="E44">
+        <v>46.1</v>
+      </c>
+      <c r="F44">
+        <v>45.4</v>
+      </c>
+      <c r="G44">
         <v>45.5</v>
       </c>
-      <c r="F44">
-        <v>43.1</v>
-      </c>
-      <c r="G44">
-        <v>41.2</v>
-      </c>
       <c r="H44">
-        <v>39.7</v>
+        <v>46.2</v>
       </c>
       <c r="I44">
-        <v>38.7</v>
+        <v>47.4</v>
       </c>
       <c r="J44">
-        <v>38.2</v>
+        <v>49.1</v>
       </c>
       <c r="K44">
-        <v>38.1</v>
+        <v>51</v>
       </c>
       <c r="L44">
-        <v>38.4</v>
+        <v>52.9</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -2207,37 +2207,37 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>46.8</v>
+        <v>44.1</v>
       </c>
       <c r="C45">
-        <v>43.3</v>
+        <v>42</v>
       </c>
       <c r="D45">
-        <v>40.2</v>
+        <v>40.9</v>
       </c>
       <c r="E45">
-        <v>37.7</v>
+        <v>41.1</v>
       </c>
       <c r="F45">
-        <v>36</v>
+        <v>42.5</v>
       </c>
       <c r="G45">
-        <v>35.2</v>
+        <v>45.2</v>
       </c>
       <c r="H45">
-        <v>35.1</v>
+        <v>48.8</v>
       </c>
       <c r="I45">
-        <v>35.9</v>
+        <v>53.2</v>
       </c>
       <c r="J45">
-        <v>37.3</v>
+        <v>58.1</v>
       </c>
       <c r="K45">
-        <v>39.1</v>
+        <v>63.1</v>
       </c>
       <c r="L45">
-        <v>41.3</v>
+        <v>67.8</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -2245,37 +2245,37 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>72.40000000000001</v>
+        <v>71.2</v>
       </c>
       <c r="C46">
-        <v>71.59999999999999</v>
+        <v>69.09999999999999</v>
       </c>
       <c r="D46">
-        <v>69.90000000000001</v>
+        <v>66.2</v>
       </c>
       <c r="E46">
-        <v>67.59999999999999</v>
+        <v>62.7</v>
       </c>
       <c r="F46">
-        <v>64.90000000000001</v>
+        <v>59.1</v>
       </c>
       <c r="G46">
-        <v>62.2</v>
+        <v>55.4</v>
       </c>
       <c r="H46">
-        <v>59.7</v>
+        <v>52.1</v>
       </c>
       <c r="I46">
-        <v>57.5</v>
+        <v>49.1</v>
       </c>
       <c r="J46">
-        <v>55.8</v>
+        <v>46.5</v>
       </c>
       <c r="K46">
-        <v>54.5</v>
+        <v>44.3</v>
       </c>
       <c r="L46">
-        <v>53.5</v>
+        <v>42.5</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -2283,37 +2283,37 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>28.6</v>
+        <v>30.7</v>
       </c>
       <c r="C47">
-        <v>30.6</v>
+        <v>33.6</v>
       </c>
       <c r="D47">
-        <v>33.2</v>
+        <v>37.1</v>
       </c>
       <c r="E47">
-        <v>36.4</v>
+        <v>41.3</v>
       </c>
       <c r="F47">
-        <v>40.2</v>
+        <v>45.8</v>
       </c>
       <c r="G47">
-        <v>44.3</v>
+        <v>50.5</v>
       </c>
       <c r="H47">
-        <v>48.5</v>
+        <v>55</v>
       </c>
       <c r="I47">
-        <v>52.4</v>
+        <v>59.1</v>
       </c>
       <c r="J47">
-        <v>55.8</v>
+        <v>62.5</v>
       </c>
       <c r="K47">
-        <v>58.6</v>
+        <v>65.09999999999999</v>
       </c>
       <c r="L47">
-        <v>60.6</v>
+        <v>66.7</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -2321,37 +2321,37 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>37.4</v>
+        <v>38.5</v>
       </c>
       <c r="C48">
-        <v>38.7</v>
+        <v>39.7</v>
       </c>
       <c r="D48">
-        <v>40.1</v>
+        <v>41</v>
       </c>
       <c r="E48">
-        <v>41.7</v>
+        <v>42.4</v>
       </c>
       <c r="F48">
-        <v>43.5</v>
+        <v>43.6</v>
       </c>
       <c r="G48">
-        <v>45.2</v>
+        <v>44.7</v>
       </c>
       <c r="H48">
-        <v>46.9</v>
+        <v>45.4</v>
       </c>
       <c r="I48">
-        <v>48.2</v>
+        <v>45.6</v>
       </c>
       <c r="J48">
-        <v>49.1</v>
+        <v>45.3</v>
       </c>
       <c r="K48">
-        <v>49.4</v>
+        <v>44.5</v>
       </c>
       <c r="L48">
-        <v>49.3</v>
+        <v>43.4</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -2359,37 +2359,37 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>36</v>
+        <v>37.6</v>
       </c>
       <c r="C49">
-        <v>37.3</v>
+        <v>39.5</v>
       </c>
       <c r="D49">
-        <v>38.9</v>
+        <v>41.8</v>
       </c>
       <c r="E49">
-        <v>40.8</v>
+        <v>44.6</v>
       </c>
       <c r="F49">
-        <v>42.9</v>
+        <v>47.5</v>
       </c>
       <c r="G49">
-        <v>45.2</v>
+        <v>50.6</v>
       </c>
       <c r="H49">
-        <v>47.3</v>
+        <v>53.5</v>
       </c>
       <c r="I49">
-        <v>49.3</v>
+        <v>56.1</v>
       </c>
       <c r="J49">
-        <v>51</v>
+        <v>58.3</v>
       </c>
       <c r="K49">
-        <v>52.2</v>
+        <v>60</v>
       </c>
       <c r="L49">
-        <v>52.9</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -2397,37 +2397,37 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>32</v>
+        <v>34.8</v>
       </c>
       <c r="C50">
-        <v>34.7</v>
+        <v>38</v>
       </c>
       <c r="D50">
-        <v>37.6</v>
+        <v>41.3</v>
       </c>
       <c r="E50">
-        <v>40.7</v>
+        <v>44.8</v>
       </c>
       <c r="F50">
-        <v>43.7</v>
+        <v>48.2</v>
       </c>
       <c r="G50">
-        <v>46.7</v>
+        <v>51.4</v>
       </c>
       <c r="H50">
-        <v>49.4</v>
+        <v>54.4</v>
       </c>
       <c r="I50">
-        <v>51.8</v>
+        <v>57</v>
       </c>
       <c r="J50">
-        <v>53.7</v>
+        <v>59.1</v>
       </c>
       <c r="K50">
-        <v>55.2</v>
+        <v>60.6</v>
       </c>
       <c r="L50">
-        <v>56.1</v>
+        <v>61.4</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -2435,37 +2435,37 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>66.09999999999999</v>
+        <v>64.8</v>
       </c>
       <c r="C51">
-        <v>64.8</v>
+        <v>62.9</v>
       </c>
       <c r="D51">
-        <v>63</v>
+        <v>60.5</v>
       </c>
       <c r="E51">
-        <v>60.7</v>
+        <v>57.9</v>
       </c>
       <c r="F51">
-        <v>58.2</v>
+        <v>54.9</v>
       </c>
       <c r="G51">
-        <v>55.4</v>
+        <v>51.7</v>
       </c>
       <c r="H51">
-        <v>52.4</v>
+        <v>48.4</v>
       </c>
       <c r="I51">
-        <v>49.3</v>
+        <v>45.1</v>
       </c>
       <c r="J51">
-        <v>46.1</v>
+        <v>41.8</v>
       </c>
       <c r="K51">
-        <v>43</v>
+        <v>38.6</v>
       </c>
       <c r="L51">
-        <v>40</v>
+        <v>35.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>